<commit_message>
Narrative Engine Importing Setup
Implemented Character Trait importing:
- Narrative Importer now can import character traits.
- Narrative Importer can now import character lists including all base data and additional trait data.
</commit_message>
<xml_diff>
--- a/Assets/StoryCSVs/TestCSVs/WholeWorkbook/Test_Narrative_Workbook.xlsx
+++ b/Assets/StoryCSVs/TestCSVs/WholeWorkbook/Test_Narrative_Workbook.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karee\Documents\GitRepo\DataGame\DataGame\Assets\StoryCSVs\TestCSVs\WholeWorkbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12791EE-FB52-4E2E-92FD-4C6D9AA3D96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC794BA-0402-4CD7-9554-3A77CAFCF42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30624" yWindow="-96" windowWidth="30912" windowHeight="16872" activeTab="2" xr2:uid="{C3FDA416-CBEF-4DA2-AAFE-8CA8E918681D}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{C3FDA416-CBEF-4DA2-AAFE-8CA8E918681D}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemTable" sheetId="1" r:id="rId1"/>
     <sheet name="Characters" sheetId="4" r:id="rId2"/>
-    <sheet name="Chatlog 1A" sheetId="2" r:id="rId3"/>
-    <sheet name="Chatlog Template" sheetId="3" r:id="rId4"/>
+    <sheet name="Locations" sheetId="5" r:id="rId3"/>
+    <sheet name="Chatlog 1A" sheetId="2" r:id="rId4"/>
+    <sheet name="Chatlog Template" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="LOCALE">Locations!$C:$C</definedName>
     <definedName name="NAMES">Characters!$B:$B</definedName>
+    <definedName name="TITLE">Locations!$C$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -76,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -174,9 +177,6 @@
     <t>PleaseDontLookForMe</t>
   </si>
   <si>
-    <t>FireCrotch</t>
-  </si>
-  <si>
     <t>Melanie</t>
   </si>
   <si>
@@ -204,6 +204,81 @@
   </si>
   <si>
     <t># This is a message. It will appear, in this chat, at 18:00 in game, time.</t>
+  </si>
+  <si>
+    <t>FlameGurl</t>
+  </si>
+  <si>
+    <t>MelMel</t>
+  </si>
+  <si>
+    <t>Xamtar</t>
+  </si>
+  <si>
+    <t>Chimicha</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>Locale</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Seppland</t>
+  </si>
+  <si>
+    <t>Nutteford</t>
+  </si>
+  <si>
+    <t>Nuttemouth</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Nuttefordshire</t>
+  </si>
+  <si>
+    <t>Nuttemyn Wells</t>
+  </si>
+  <si>
+    <t>Oxeley</t>
+  </si>
+  <si>
+    <t>Antesbury</t>
+  </si>
+  <si>
+    <t>Medium seaside village, contains aquatic college</t>
+  </si>
+  <si>
+    <t>Small village. Mostly retirees &amp; nursing homes</t>
+  </si>
+  <si>
+    <t>County Capital. Medium size town. River Nutte runs directly through</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern suburb of Nutteford. Middle-upper class. </t>
+  </si>
+  <si>
+    <t>Northern suburb of Nutteford. Working-middle class.</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>LOCATION</t>
+  </si>
+  <si>
+    <t>BIRTHPLACE</t>
+  </si>
+  <si>
+    <t>EDUCATION</t>
+  </si>
+  <si>
+    <t>OCCUPATION</t>
   </si>
 </sst>
 </file>
@@ -260,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -275,6 +350,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -292,10 +371,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3413,32 +3488,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D9048A-2A84-4417-B532-6BF062B3741B}">
-  <dimension ref="A1:D196"/>
+  <dimension ref="A1:H196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3449,7 +3540,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3460,7 +3551,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3468,74 +3559,83 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4438,6 +4538,134 @@
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F201" xr:uid="{962003AE-3AD2-4D2B-A8BA-0550CA029FB4}">
+      <formula1>LOCALE</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB52E31-61D3-421D-9695-39338102F5F1}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="7">
+        <v>7000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="7">
+        <v>2000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="7">
+        <v>30000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="7">
+        <v>3000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="7">
+        <v>8000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -4445,12 +4673,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75D9D40-B82B-4836-B9A6-01E5F8AA0E57}">
   <dimension ref="A1:D720"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4475,7 +4703,7 @@
         <v>0.75</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4515,7 +4743,7 @@
         <v>0.75347222222222199</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4539,7 +4767,7 @@
         <v>0.75555555555555598</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4569,7 +4797,7 @@
         <v>0.75763888888888897</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4593,7 +4821,7 @@
         <v>0.75972222222222197</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -4601,7 +4829,7 @@
         <v>0.76041666666666696</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -7888,7 +8116,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01909B1B-44B6-4544-B68A-EC97546CA38A}">
   <dimension ref="A1:D601"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updates to narrative importing.
Narrative importing pipeline now covers traits and characters properly.

Added vacuum tube & sockets for socketing character punchcards.
</commit_message>
<xml_diff>
--- a/Assets/StoryCSVs/TestCSVs/WholeWorkbook/Test_Narrative_Workbook.xlsx
+++ b/Assets/StoryCSVs/TestCSVs/WholeWorkbook/Test_Narrative_Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karimajouz/Documents/GitRepo/DataGame/DataGame/Assets/StoryCSVs/TestCSVs/WholeWorkbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87006BB2-8401-FD46-A5DF-A6E57F24B067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52293EE7-E288-984E-ADDD-59EC42C64F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" activeTab="4" xr2:uid="{C3FDA416-CBEF-4DA2-AAFE-8CA8E918681D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{C3FDA416-CBEF-4DA2-AAFE-8CA8E918681D}"/>
   </bookViews>
   <sheets>
     <sheet name="TraitTable" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="122">
   <si>
     <t>ID</t>
   </si>
@@ -232,9 +232,6 @@
     <t>LOCATION</t>
   </si>
   <si>
-    <t>BIRTHPLACE</t>
-  </si>
-  <si>
     <t>EDUCATION</t>
   </si>
   <si>
@@ -245,15 +242,6 @@
   </si>
   <si>
     <t>WebID</t>
-  </si>
-  <si>
-    <t>EMPLOYMENT STATUS</t>
-  </si>
-  <si>
-    <t>OCCUPATION FIELD</t>
-  </si>
-  <si>
-    <t>GENDER IDENTITY</t>
   </si>
   <si>
     <t>SEXUALITY</t>
@@ -370,9 +358,6 @@
     <t>Education</t>
   </si>
   <si>
-    <t>LOCATIONS</t>
-  </si>
-  <si>
     <t>As the first item in this spreadsheet this is the initial forum post</t>
   </si>
   <si>
@@ -453,6 +438,30 @@
   </si>
   <si>
     <t># The muffin man.</t>
+  </si>
+  <si>
+    <t>EMPLOYMENT_STATUS</t>
+  </si>
+  <si>
+    <t>OCCUPATION_FIELD</t>
+  </si>
+  <si>
+    <t>GENDER_IDENTITY</t>
+  </si>
+  <si>
+    <t>LOCATION_CURRENT</t>
+  </si>
+  <si>
+    <t>LOCATION_BIRTHPLACE</t>
+  </si>
+  <si>
+    <t>GENDER</t>
+  </si>
+  <si>
+    <t>OCCUPATION</t>
+  </si>
+  <si>
+    <t>EMPLOYMENT</t>
   </si>
 </sst>
 </file>
@@ -867,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338823B8-C032-4C47-BD81-E46255195D8B}">
   <dimension ref="A1:G550"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -887,22 +896,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>53</v>
+        <v>120</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>93</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -910,19 +919,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
         <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" t="s">
-        <v>60</v>
       </c>
       <c r="G2" t="s">
         <v>35</v>
@@ -933,19 +942,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
         <v>61</v>
-      </c>
-      <c r="C3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" t="s">
-        <v>65</v>
       </c>
       <c r="G3" t="s">
         <v>38</v>
@@ -956,19 +965,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
         <v>66</v>
-      </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -976,16 +985,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G5" t="s">
         <v>39</v>
@@ -996,16 +1005,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G6" t="s">
         <v>40</v>
@@ -1016,13 +1025,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1030,13 +1039,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1044,10 +1053,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1055,10 +1064,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1066,10 +1075,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1077,10 +1086,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -3783,7 +3792,7 @@
   <dimension ref="A1:L196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3807,34 +3816,34 @@
         <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -3845,7 +3854,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3854,25 +3863,25 @@
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G2" s="8">
         <v>27004</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="K2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -3883,7 +3892,7 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -3892,25 +3901,25 @@
         <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G3" s="8">
         <v>26505</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="K3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -3921,7 +3930,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -3936,19 +3945,19 @@
         <v>26894</v>
       </c>
       <c r="H4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -3974,19 +3983,19 @@
         <v>33298</v>
       </c>
       <c r="H5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -4006,25 +4015,25 @@
         <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G6" s="8">
         <v>31084</v>
       </c>
       <c r="H6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -4050,19 +4059,19 @@
         <v>34772</v>
       </c>
       <c r="H7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="K7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -4070,10 +4079,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -4088,19 +4097,19 @@
         <v>31980</v>
       </c>
       <c r="H8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -4108,10 +4117,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -4126,19 +4135,19 @@
         <v>31981</v>
       </c>
       <c r="H9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -4146,10 +4155,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -4164,19 +4173,19 @@
         <v>31982</v>
       </c>
       <c r="H10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -5215,7 +5224,7 @@
         <v>30000</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -8704,7 +8713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28CF1F1-F6C4-5344-AA49-CF5550407A65}">
   <dimension ref="A1:D601"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -8717,10 +8726,10 @@
     <row r="1" spans="1:4" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D1" s="4"/>
     </row>
@@ -8809,7 +8818,7 @@
         <v>0.75694444444444398</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -8820,7 +8829,7 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -8829,7 +8838,7 @@
         <v>0.75833333333333297</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -8840,7 +8849,7 @@
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -8849,7 +8858,7 @@
         <v>0.75972222222222197</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -8860,7 +8869,7 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -8869,7 +8878,7 @@
         <v>0.76111111111111096</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -8880,7 +8889,7 @@
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -8889,7 +8898,7 @@
         <v>0.76249999999999996</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -8900,7 +8909,7 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -8909,7 +8918,7 @@
         <v>0.76388888888888895</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -8920,7 +8929,7 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -18428,7 +18437,7 @@
         <v>0.75</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -18456,7 +18465,7 @@
         <v>0.75347222222222199</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -18469,7 +18478,7 @@
         <v>0.75486111111111098</v>
       </c>
       <c r="D9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -18477,7 +18486,7 @@
         <v>0.75555555555555598</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -18485,7 +18494,7 @@
         <v>0.75624999999999998</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Data input fields can now take socketed trait cards
</commit_message>
<xml_diff>
--- a/Assets/StoryCSVs/TestCSVs/WholeWorkbook/Test_Narrative_Workbook.xlsx
+++ b/Assets/StoryCSVs/TestCSVs/WholeWorkbook/Test_Narrative_Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karimajouz/Documents/GitRepo/DataGame/DataGame/Assets/StoryCSVs/TestCSVs/WholeWorkbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52293EE7-E288-984E-ADDD-59EC42C64F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECA6019-94C3-C144-B6C8-B2AC6449A8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{C3FDA416-CBEF-4DA2-AAFE-8CA8E918681D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" activeTab="3" xr2:uid="{C3FDA416-CBEF-4DA2-AAFE-8CA8E918681D}"/>
   </bookViews>
   <sheets>
     <sheet name="TraitTable" sheetId="1" r:id="rId1"/>
@@ -87,15 +87,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="121">
   <si>
     <t>ID</t>
   </si>
   <si>
     <t>John</t>
-  </si>
-  <si>
-    <t>David</t>
   </si>
   <si>
     <t>Amy</t>
@@ -876,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338823B8-C032-4C47-BD81-E46255195D8B}">
   <dimension ref="A1:G550"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -896,22 +893,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -919,22 +916,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
         <v>52</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>53</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>54</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>55</v>
       </c>
-      <c r="F2" t="s">
-        <v>56</v>
-      </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -942,22 +939,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
         <v>57</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>58</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>59</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>60</v>
       </c>
-      <c r="F3" t="s">
-        <v>61</v>
-      </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -965,19 +962,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>63</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>64</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>65</v>
-      </c>
-      <c r="G4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -985,19 +982,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
         <v>67</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>68</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>69</v>
       </c>
-      <c r="F5" t="s">
-        <v>70</v>
-      </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1005,19 +1002,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
         <v>71</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>72</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>73</v>
       </c>
-      <c r="F6" t="s">
-        <v>74</v>
-      </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1025,13 +1022,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" t="s">
         <v>75</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>76</v>
-      </c>
-      <c r="D7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1039,13 +1036,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
         <v>78</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>79</v>
-      </c>
-      <c r="D8" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1053,10 +1050,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" t="s">
         <v>81</v>
-      </c>
-      <c r="D9" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1064,10 +1061,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" t="s">
         <v>83</v>
-      </c>
-      <c r="D10" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1075,10 +1072,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" t="s">
         <v>85</v>
-      </c>
-      <c r="D11" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1086,10 +1083,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" t="s">
         <v>87</v>
-      </c>
-      <c r="D12" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -3813,37 +3810,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -3854,34 +3851,34 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G2" s="8">
         <v>27004</v>
       </c>
       <c r="H2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" t="s">
         <v>62</v>
       </c>
-      <c r="I2" t="s">
-        <v>63</v>
-      </c>
       <c r="J2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -3889,37 +3886,37 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G3" s="8">
         <v>26505</v>
       </c>
       <c r="H3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" t="s">
         <v>55</v>
-      </c>
-      <c r="L3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -3927,37 +3924,37 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" s="8">
         <v>26894</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" t="s">
         <v>72</v>
       </c>
-      <c r="J4" t="s">
-        <v>73</v>
-      </c>
       <c r="K4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -3965,37 +3962,37 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="8">
         <v>33298</v>
       </c>
       <c r="H5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" t="s">
         <v>68</v>
       </c>
-      <c r="J5" t="s">
-        <v>69</v>
-      </c>
       <c r="K5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -4003,37 +4000,37 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G6" s="8">
         <v>31084</v>
       </c>
       <c r="H6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L6" t="s">
         <v>55</v>
-      </c>
-      <c r="L6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -4041,37 +4038,37 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
         <v>39</v>
-      </c>
-      <c r="F7" t="s">
-        <v>40</v>
       </c>
       <c r="G7" s="8">
         <v>34772</v>
       </c>
       <c r="H7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" t="s">
         <v>79</v>
       </c>
-      <c r="J7" t="s">
-        <v>80</v>
-      </c>
       <c r="K7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -4079,37 +4076,37 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
         <v>95</v>
-      </c>
-      <c r="C8" t="s">
-        <v>96</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" s="8">
         <v>31980</v>
       </c>
       <c r="H8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -4117,37 +4114,37 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" s="8">
         <v>31981</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K9" t="s">
+        <v>54</v>
+      </c>
+      <c r="L9" t="s">
         <v>55</v>
-      </c>
-      <c r="L9" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -4155,37 +4152,37 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10">
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G10" s="8">
         <v>31982</v>
       </c>
       <c r="H10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J10" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" t="s">
+        <v>54</v>
+      </c>
+      <c r="L10" t="s">
         <v>73</v>
-      </c>
-      <c r="K10" t="s">
-        <v>55</v>
-      </c>
-      <c r="L10" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -5161,104 +5158,104 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="7">
         <v>7000</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
         <v>37</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
       </c>
       <c r="D3" s="7">
         <v>2000</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
         <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
       </c>
       <c r="D4" s="7">
         <v>30000</v>
       </c>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="7">
         <v>3000</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="7">
         <v>8000</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -5270,8 +5267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75D9D40-B82B-4836-B9A6-01E5F8AA0E57}">
   <dimension ref="A1:D720"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5285,10 +5282,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -5296,7 +5293,7 @@
         <v>0.75</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -5304,7 +5301,7 @@
         <v>0.75069444444444444</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -5312,7 +5309,7 @@
         <v>0.75138888888888899</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -5320,7 +5317,7 @@
         <v>0.75208333333333299</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -5328,7 +5325,7 @@
         <v>0.75277777777777799</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -5336,7 +5333,7 @@
         <v>0.75347222222222199</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -5344,7 +5341,7 @@
         <v>0.75416666666666698</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -5352,7 +5349,7 @@
         <v>0.75486111111111098</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -5360,7 +5357,7 @@
         <v>0.75555555555555598</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -5368,7 +5365,7 @@
         <v>0.75624999999999998</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -5376,13 +5373,13 @@
         <v>0.75694444444444398</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -5390,7 +5387,7 @@
         <v>0.75763888888888897</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -5398,7 +5395,7 @@
         <v>0.75833333333333297</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -5406,7 +5403,7 @@
         <v>0.75902777777777797</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -5414,7 +5411,7 @@
         <v>0.75972222222222197</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -5422,7 +5419,7 @@
         <v>0.76041666666666696</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -8714,7 +8711,7 @@
   <dimension ref="A1:D601"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8726,10 +8723,10 @@
     <row r="1" spans="1:4" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="D1" s="4"/>
     </row>
@@ -8818,7 +8815,7 @@
         <v>0.75694444444444398</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -8829,7 +8826,7 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -8838,7 +8835,7 @@
         <v>0.75833333333333297</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -8849,7 +8846,7 @@
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -8858,7 +8855,7 @@
         <v>0.75972222222222197</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -8869,7 +8866,7 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -8878,7 +8875,7 @@
         <v>0.76111111111111096</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -8889,7 +8886,7 @@
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -8898,7 +8895,7 @@
         <v>0.76249999999999996</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -8909,7 +8906,7 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -8918,7 +8915,7 @@
         <v>0.76388888888888895</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -8929,7 +8926,7 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -13584,13 +13581,13 @@
     <row r="1" spans="1:4" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -18426,10 +18423,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -18437,7 +18434,7 @@
         <v>0.75</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -18465,7 +18462,7 @@
         <v>0.75347222222222199</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -18478,7 +18475,7 @@
         <v>0.75486111111111098</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -18486,7 +18483,7 @@
         <v>0.75555555555555598</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -18494,7 +18491,7 @@
         <v>0.75624999999999998</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Split flap display works closer to intended usage
Need to manage character insertion
Need to test deletion from the middle of the string properly at full-screen scale.
</commit_message>
<xml_diff>
--- a/Assets/StoryCSVs/TestCSVs/WholeWorkbook/Test_Narrative_Workbook.xlsx
+++ b/Assets/StoryCSVs/TestCSVs/WholeWorkbook/Test_Narrative_Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karimajouz/Documents/GitRepo/DataGame/DataGame/Assets/StoryCSVs/TestCSVs/WholeWorkbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC3AA44-EA2E-704E-8F86-6E65C865D851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0FA8E3-39E5-F44D-8176-67AAD62A402A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{C3FDA416-CBEF-4DA2-AAFE-8CA8E918681D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" activeTab="7" xr2:uid="{C3FDA416-CBEF-4DA2-AAFE-8CA8E918681D}"/>
   </bookViews>
   <sheets>
     <sheet name="TraitTable" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Chatlog MuffinMan" sheetId="7" r:id="rId5"/>
     <sheet name="Chatlog Template" sheetId="3" r:id="rId6"/>
     <sheet name="ForumPostTemplate" sheetId="6" r:id="rId7"/>
+    <sheet name="Feedback" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="CHARNAME">Characters!$B$2:$B$201</definedName>
@@ -87,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="141">
   <si>
     <t>ID</t>
   </si>
@@ -459,6 +460,66 @@
   </si>
   <si>
     <t>EMPLOYMENT</t>
+  </si>
+  <si>
+    <t>What's the twist?</t>
+  </si>
+  <si>
+    <t>What's the flavour?</t>
+  </si>
+  <si>
+    <t>Aesthetic</t>
+  </si>
+  <si>
+    <t>Visuals</t>
+  </si>
+  <si>
+    <t>Culture</t>
+  </si>
+  <si>
+    <t>90s Theme,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Corporate Office Culture</t>
+  </si>
+  <si>
+    <t>Late Stage Capitalism</t>
+  </si>
+  <si>
+    <t>What is the flavour?</t>
+  </si>
+  <si>
+    <t>What is the twist?</t>
+  </si>
+  <si>
+    <t>Unless I want players to feel the suffocating hopelessness of late stage capitalism…</t>
+  </si>
+  <si>
+    <t>If I want to take it further than that I should be thinking about narrative catharsis</t>
+  </si>
+  <si>
+    <t>How do I give the player the ending that makes sense/give them a sense of accomplishment</t>
+  </si>
+  <si>
+    <t>Do I give them a moment of release? What does that look like?</t>
+  </si>
+  <si>
+    <t>The Caution:</t>
+  </si>
+  <si>
+    <t>What I've described narratively/genre-wise is a 1980s narrative dystopia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very popular genre - how do I use that genre as a basis that I can build off of </t>
+  </si>
+  <si>
+    <t>Needs to be new, unique, and innovate there</t>
+  </si>
+  <si>
+    <t>Success here comes from finding uniqueness within the genre</t>
+  </si>
+  <si>
+    <t>Nicks Comments</t>
   </si>
 </sst>
 </file>
@@ -873,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338823B8-C032-4C47-BD81-E46255195D8B}">
   <dimension ref="A1:G550"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5148,7 +5209,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8714,13 +8775,15 @@
   <dimension ref="A1:D601"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="57.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -21812,4 +21875,108 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01092DD-DEEC-1C4D-8992-87670F9AD878}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.1640625" customWidth="1"/>
+    <col min="3" max="3" width="43.83203125" customWidth="1"/>
+    <col min="4" max="4" width="48" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="69.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>